<commit_message>
[+] Add more logging [+] const rand [+] racalc Omega and sigma [~] calcQuantile rework. Now named calcF(sigma2, sigmaDash2)
</commit_message>
<xml_diff>
--- a/Лист Microsoft Excel.xlsx
+++ b/Лист Microsoft Excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>x1</t>
   </si>
@@ -28,6 +28,33 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>yDash</t>
+  </si>
+  <si>
+    <t>y-yDash</t>
+  </si>
+  <si>
+    <t>Столбец1</t>
+  </si>
+  <si>
+    <t>Столбец2</t>
+  </si>
+  <si>
+    <t>Столбец3</t>
+  </si>
+  <si>
+    <t>Столбец4</t>
+  </si>
+  <si>
+    <t>Столбец5</t>
+  </si>
+  <si>
+    <t>Столбец6</t>
   </si>
 </sst>
 </file>
@@ -54,7 +81,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -77,11 +104,72 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -89,17 +177,193 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="11">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -110,6 +374,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Таблица4" displayName="Таблица4" ref="G8:L34" totalsRowShown="0" headerRowDxfId="10" dataDxfId="0" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+  <autoFilter ref="G8:L34"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Столбец1" dataDxfId="6"/>
+    <tableColumn id="2" name="Столбец2" dataDxfId="5"/>
+    <tableColumn id="3" name="Столбец3" dataDxfId="4"/>
+    <tableColumn id="4" name="Столбец4" dataDxfId="3"/>
+    <tableColumn id="5" name="Столбец5" dataDxfId="2"/>
+    <tableColumn id="6" name="Столбец6" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -378,31 +657,57 @@
   <dimension ref="G8:P45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:I33"/>
+      <selection activeCell="G9" sqref="G9:L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="7.109375" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" customWidth="1"/>
+    <col min="9" max="9" width="6.109375" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" customWidth="1"/>
+    <col min="11" max="11" width="8.44140625" customWidth="1"/>
+    <col min="12" max="12" width="9" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="8" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="7:16" x14ac:dyDescent="0.3">
+      <c r="G9" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" s="3" t="s">
+      <c r="H9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G9" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H9" s="3">
-        <v>-1</v>
-      </c>
-      <c r="I9" s="4">
-        <v>5.0847562308520704</v>
+      <c r="J9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>0</v>
@@ -415,15 +720,25 @@
       </c>
     </row>
     <row r="10" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G10" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H10" s="3">
-        <v>-0.5</v>
-      </c>
-      <c r="I10" s="4">
-        <v>2.7870911690737099</v>
-      </c>
+      <c r="G10" s="10">
+        <v>-1</v>
+      </c>
+      <c r="H10" s="10">
+        <v>-1</v>
+      </c>
+      <c r="I10" s="11">
+        <v>6.0648682029392802</v>
+      </c>
+      <c r="J10" s="11">
+        <v>5.1839641188334902</v>
+      </c>
+      <c r="K10" s="11">
+        <v>5.5454560312107501</v>
+      </c>
+      <c r="L10" s="11">
+        <v>0.51941217172853105</v>
+      </c>
+      <c r="M10" s="4"/>
       <c r="N10" s="1">
         <v>-1</v>
       </c>
@@ -435,15 +750,25 @@
       </c>
     </row>
     <row r="11" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H11" s="3">
-        <v>0</v>
-      </c>
-      <c r="I11" s="4">
-        <v>0.68743794259917201</v>
-      </c>
+      <c r="G11" s="10">
+        <v>-1</v>
+      </c>
+      <c r="H11" s="10">
+        <v>-0.5</v>
+      </c>
+      <c r="I11" s="11">
+        <v>2.7423360840721598</v>
+      </c>
+      <c r="J11" s="11">
+        <v>2.5722651734247499</v>
+      </c>
+      <c r="K11" s="11">
+        <v>2.6566677316397</v>
+      </c>
+      <c r="L11" s="11">
+        <v>8.5668352432464998E-2</v>
+      </c>
+      <c r="M11" s="4"/>
       <c r="N11" s="1">
         <v>-1</v>
       </c>
@@ -455,15 +780,25 @@
       </c>
     </row>
     <row r="12" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G12" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H12" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="I12" s="4">
-        <v>1.85701909655778</v>
-      </c>
+      <c r="G12" s="10">
+        <v>-1</v>
+      </c>
+      <c r="H12" s="10">
+        <v>0</v>
+      </c>
+      <c r="I12" s="11">
+        <v>1.18941489849354</v>
+      </c>
+      <c r="J12" s="11">
+        <v>1.00262374853703</v>
+      </c>
+      <c r="K12" s="11">
+        <v>0.89663608523288396</v>
+      </c>
+      <c r="L12" s="11">
+        <v>0.29277881326066402</v>
+      </c>
+      <c r="M12" s="4"/>
       <c r="N12" s="1">
         <v>-1</v>
       </c>
@@ -475,15 +810,25 @@
       </c>
     </row>
     <row r="13" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H13" s="3">
-        <v>1</v>
-      </c>
-      <c r="I13" s="4">
-        <v>5.2210727249308002</v>
-      </c>
+      <c r="G13" s="10">
+        <v>-1</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I13" s="11">
+        <v>1.9998711834116001</v>
+      </c>
+      <c r="J13" s="11">
+        <v>1.93298232364932</v>
+      </c>
+      <c r="K13" s="11">
+        <v>2.0810303118314102</v>
+      </c>
+      <c r="L13" s="11">
+        <v>-8.1159128419811405E-2</v>
+      </c>
+      <c r="M13" s="4"/>
       <c r="N13" s="1">
         <v>-1</v>
       </c>
@@ -495,15 +840,25 @@
       </c>
     </row>
     <row r="14" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G14" s="3">
-        <v>-0.5</v>
-      </c>
-      <c r="H14" s="3">
-        <v>-1</v>
-      </c>
-      <c r="I14" s="4">
-        <v>3.4111998898281999</v>
-      </c>
+      <c r="G14" s="10">
+        <v>-1</v>
+      </c>
+      <c r="H14" s="10">
+        <v>1</v>
+      </c>
+      <c r="I14" s="11">
+        <v>4.7420320993609097</v>
+      </c>
+      <c r="J14" s="11">
+        <v>4.8212833782405804</v>
+      </c>
+      <c r="K14" s="11">
+        <v>5.2188828941362901</v>
+      </c>
+      <c r="L14" s="11">
+        <v>-0.47685079477537501</v>
+      </c>
+      <c r="M14" s="4"/>
       <c r="N14" s="1">
         <v>-1</v>
       </c>
@@ -515,15 +870,25 @@
       </c>
     </row>
     <row r="15" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G15" s="3">
+      <c r="G15" s="10">
         <v>-0.5</v>
       </c>
-      <c r="H15" s="3">
-        <v>-0.5</v>
-      </c>
-      <c r="I15" s="4">
-        <v>2.1633998776597099</v>
-      </c>
+      <c r="H15" s="10">
+        <v>-1</v>
+      </c>
+      <c r="I15" s="11">
+        <v>4.8661400124775298</v>
+      </c>
+      <c r="J15" s="11">
+        <v>4.18266388779743</v>
+      </c>
+      <c r="K15" s="11">
+        <v>4.3955261110202697</v>
+      </c>
+      <c r="L15" s="11">
+        <v>0.47061390145726201</v>
+      </c>
+      <c r="M15" s="4"/>
       <c r="N15" s="1">
         <v>-1</v>
       </c>
@@ -535,15 +900,25 @@
       </c>
     </row>
     <row r="16" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G16" s="3">
+      <c r="G16" s="10">
         <v>-0.5</v>
       </c>
-      <c r="H16" s="3">
-        <v>0</v>
-      </c>
-      <c r="I16" s="4">
-        <v>4.0193011775815296E-3</v>
-      </c>
+      <c r="H16" s="10">
+        <v>-0.5</v>
+      </c>
+      <c r="I16" s="11">
+        <v>1.7687210953550101</v>
+      </c>
+      <c r="J16" s="11">
+        <v>1.82096494238869</v>
+      </c>
+      <c r="K16" s="11">
+        <v>1.85756740359173</v>
+      </c>
+      <c r="L16" s="11">
+        <v>-8.8846308236726304E-2</v>
+      </c>
+      <c r="M16" s="4"/>
       <c r="N16" s="1">
         <v>-0.6</v>
       </c>
@@ -555,15 +930,25 @@
       </c>
     </row>
     <row r="17" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G17" s="3">
+      <c r="G17" s="10">
         <v>-0.5</v>
       </c>
-      <c r="H17" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="I17" s="4">
-        <v>1.3283733100215001</v>
-      </c>
+      <c r="H17" s="10">
+        <v>0</v>
+      </c>
+      <c r="I17" s="11">
+        <v>0.46561384912399301</v>
+      </c>
+      <c r="J17" s="11">
+        <v>0.50132351750097703</v>
+      </c>
+      <c r="K17" s="11">
+        <v>0.44836534932743299</v>
+      </c>
+      <c r="L17" s="11">
+        <v>1.7248499796560499E-2</v>
+      </c>
+      <c r="M17" s="4"/>
       <c r="N17" s="1">
         <v>-0.6</v>
       </c>
@@ -575,15 +960,25 @@
       </c>
     </row>
     <row r="18" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G18" s="3">
+      <c r="G18" s="10">
         <v>-0.5</v>
       </c>
-      <c r="H18" s="3">
-        <v>1</v>
-      </c>
-      <c r="I18" s="4">
-        <v>3.7750928348253101</v>
-      </c>
+      <c r="H18" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I18" s="11">
+        <v>0.41299690846770698</v>
+      </c>
+      <c r="J18" s="11">
+        <v>1.1816820926132601</v>
+      </c>
+      <c r="K18" s="11">
+        <v>1.2819299837834499</v>
+      </c>
+      <c r="L18" s="11">
+        <v>-0.86893307531574204</v>
+      </c>
+      <c r="M18" s="4"/>
       <c r="N18" s="1">
         <v>-0.6</v>
       </c>
@@ -595,15 +990,25 @@
       </c>
     </row>
     <row r="19" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G19" s="3">
-        <v>0</v>
-      </c>
-      <c r="H19" s="3">
-        <v>-1</v>
-      </c>
-      <c r="I19" s="4">
-        <v>3.02842025693261</v>
-      </c>
+      <c r="G19" s="10">
+        <v>-0.5</v>
+      </c>
+      <c r="H19" s="10">
+        <v>1</v>
+      </c>
+      <c r="I19" s="11">
+        <v>3.8606055996247601</v>
+      </c>
+      <c r="J19" s="11">
+        <v>3.8199831472045198</v>
+      </c>
+      <c r="K19" s="11">
+        <v>4.0689529739458097</v>
+      </c>
+      <c r="L19" s="11">
+        <v>-0.208347374321047</v>
+      </c>
+      <c r="M19" s="4"/>
       <c r="N19" s="1">
         <v>-0.6</v>
       </c>
@@ -615,15 +1020,25 @@
       </c>
     </row>
     <row r="20" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G20" s="3">
+      <c r="G20" s="10">
         <v>0</v>
       </c>
-      <c r="H20" s="3">
-        <v>-0.5</v>
-      </c>
-      <c r="I20" s="4">
-        <v>0.79131000773698701</v>
-      </c>
+      <c r="H20" s="10">
+        <v>-1</v>
+      </c>
+      <c r="I20" s="11">
+        <v>3.0409261824260798</v>
+      </c>
+      <c r="J20" s="11">
+        <v>3.18134037029645</v>
+      </c>
+      <c r="K20" s="11">
+        <v>3.24550157740781</v>
+      </c>
+      <c r="L20" s="11">
+        <v>-0.204575394981726</v>
+      </c>
+      <c r="M20" s="4"/>
       <c r="N20" s="1">
         <v>-0.6</v>
       </c>
@@ -635,15 +1050,25 @@
       </c>
     </row>
     <row r="21" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G21" s="3">
+      <c r="G21" s="10">
         <v>0</v>
       </c>
-      <c r="H21" s="3">
-        <v>0</v>
-      </c>
-      <c r="I21" s="4">
-        <v>0.53148143515531399</v>
-      </c>
+      <c r="H21" s="10">
+        <v>-0.5</v>
+      </c>
+      <c r="I21" s="11">
+        <v>1.2174839451719</v>
+      </c>
+      <c r="J21" s="11">
+        <v>1.06964142488771</v>
+      </c>
+      <c r="K21" s="11">
+        <v>1.05837246212178</v>
+      </c>
+      <c r="L21" s="11">
+        <v>0.15911148305012099</v>
+      </c>
+      <c r="M21" s="4"/>
       <c r="N21" s="1">
         <v>-0.6</v>
       </c>
@@ -655,15 +1080,25 @@
       </c>
     </row>
     <row r="22" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G22" s="3">
+      <c r="G22" s="10">
         <v>0</v>
       </c>
-      <c r="H22" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="I22" s="4">
-        <v>0.38990152271613099</v>
-      </c>
+      <c r="H22" s="10">
+        <v>0</v>
+      </c>
+      <c r="I22" s="11">
+        <v>0.86679533639275197</v>
+      </c>
+      <c r="J22" s="11">
+        <v>0</v>
+      </c>
+      <c r="K22" s="11">
+        <v>0</v>
+      </c>
+      <c r="L22" s="11">
+        <v>0.86679533639275197</v>
+      </c>
+      <c r="M22" s="4"/>
       <c r="N22" s="1">
         <v>-0.19999999999999901</v>
       </c>
@@ -675,15 +1110,25 @@
       </c>
     </row>
     <row r="23" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G23" s="3">
+      <c r="G23" s="10">
         <v>0</v>
       </c>
-      <c r="H23" s="3">
-        <v>1</v>
-      </c>
-      <c r="I23" s="4">
-        <v>2.9071299067152401</v>
-      </c>
+      <c r="H23" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I23" s="11">
+        <v>1.04854102162524</v>
+      </c>
+      <c r="J23" s="11">
+        <v>0.43035857511228698</v>
+      </c>
+      <c r="K23" s="11">
+        <v>0.48273504231350101</v>
+      </c>
+      <c r="L23" s="11">
+        <v>0.56580597931174403</v>
+      </c>
+      <c r="M23" s="4"/>
       <c r="N23" s="1">
         <v>-0.19999999999999901</v>
       </c>
@@ -695,15 +1140,25 @@
       </c>
     </row>
     <row r="24" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G24" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="H24" s="3">
-        <v>-1</v>
-      </c>
-      <c r="I24" s="4">
-        <v>3.7612520698697698</v>
-      </c>
+      <c r="G24" s="10">
+        <v>0</v>
+      </c>
+      <c r="H24" s="10">
+        <v>1</v>
+      </c>
+      <c r="I24" s="11">
+        <v>2.7616912660708102</v>
+      </c>
+      <c r="J24" s="11">
+        <v>2.8186596297035398</v>
+      </c>
+      <c r="K24" s="11">
+        <v>2.9189284403333402</v>
+      </c>
+      <c r="L24" s="11">
+        <v>-0.157237174262534</v>
+      </c>
+      <c r="M24" s="4"/>
       <c r="N24" s="1">
         <v>-0.19999999999999901</v>
       </c>
@@ -715,15 +1170,25 @@
       </c>
     </row>
     <row r="25" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G25" s="3">
+      <c r="G25" s="10">
         <v>0.5</v>
       </c>
-      <c r="H25" s="3">
-        <v>-0.5</v>
-      </c>
-      <c r="I25" s="4">
-        <v>1.3911937364447</v>
-      </c>
+      <c r="H25" s="10">
+        <v>-1</v>
+      </c>
+      <c r="I25" s="11">
+        <v>4.0879182107373904</v>
+      </c>
+      <c r="J25" s="11">
+        <v>4.18001685279547</v>
+      </c>
+      <c r="K25" s="11">
+        <v>4.3847711492626704</v>
+      </c>
+      <c r="L25" s="11">
+        <v>-0.296852938525278</v>
+      </c>
+      <c r="M25" s="4"/>
       <c r="N25" s="1">
         <v>-0.19999999999999901</v>
       </c>
@@ -735,15 +1200,25 @@
       </c>
     </row>
     <row r="26" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G26" s="3">
+      <c r="G26" s="10">
         <v>0.5</v>
       </c>
-      <c r="H26" s="3">
-        <v>0</v>
-      </c>
-      <c r="I26" s="4">
-        <v>0.45959838453077401</v>
-      </c>
+      <c r="H26" s="10">
+        <v>-0.5</v>
+      </c>
+      <c r="I26" s="11">
+        <v>1.8217787544011499</v>
+      </c>
+      <c r="J26" s="11">
+        <v>1.8183179073867299</v>
+      </c>
+      <c r="K26" s="11">
+        <v>1.8468124418341301</v>
+      </c>
+      <c r="L26" s="11">
+        <v>-2.50336874329848E-2</v>
+      </c>
+      <c r="M26" s="4"/>
       <c r="N26" s="1">
         <v>-0.19999999999999901</v>
       </c>
@@ -755,15 +1230,25 @@
       </c>
     </row>
     <row r="27" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G27" s="3">
+      <c r="G27" s="10">
         <v>0.5</v>
       </c>
-      <c r="H27" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="I27" s="4">
-        <v>0.71310263237517901</v>
-      </c>
+      <c r="H27" s="10">
+        <v>0</v>
+      </c>
+      <c r="I27" s="11">
+        <v>-0.36575428512761299</v>
+      </c>
+      <c r="J27" s="11">
+        <v>0.49867648249902202</v>
+      </c>
+      <c r="K27" s="11">
+        <v>0.437610387569832</v>
+      </c>
+      <c r="L27" s="11">
+        <v>-0.80336467269744605</v>
+      </c>
+      <c r="M27" s="4"/>
       <c r="N27" s="1">
         <v>-0.19999999999999901</v>
       </c>
@@ -775,15 +1260,25 @@
       </c>
     </row>
     <row r="28" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G28" s="3">
+      <c r="G28" s="10">
         <v>0.5</v>
       </c>
-      <c r="H28" s="3">
-        <v>1</v>
-      </c>
-      <c r="I28" s="4">
-        <v>4.0364397512265002</v>
-      </c>
+      <c r="H28" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I28" s="11">
+        <v>1.69313395161355</v>
+      </c>
+      <c r="J28" s="11">
+        <v>1.1790350576113</v>
+      </c>
+      <c r="K28" s="11">
+        <v>1.27117502202584</v>
+      </c>
+      <c r="L28" s="11">
+        <v>0.42195892958770298</v>
+      </c>
+      <c r="M28" s="4"/>
       <c r="N28" s="1">
         <v>0.2</v>
       </c>
@@ -795,15 +1290,25 @@
       </c>
     </row>
     <row r="29" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G29" s="3">
-        <v>1</v>
-      </c>
-      <c r="H29" s="3">
-        <v>-1</v>
-      </c>
-      <c r="I29" s="4">
-        <v>5.1039056498513897</v>
-      </c>
+      <c r="G29" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="H29" s="10">
+        <v>1</v>
+      </c>
+      <c r="I29" s="11">
+        <v>4.4064776119840001</v>
+      </c>
+      <c r="J29" s="11">
+        <v>3.8173361122025602</v>
+      </c>
+      <c r="K29" s="11">
+        <v>4.0581980121882104</v>
+      </c>
+      <c r="L29" s="11">
+        <v>0.34827959979579298</v>
+      </c>
+      <c r="M29" s="4"/>
       <c r="N29" s="1">
         <v>0.2</v>
       </c>
@@ -815,15 +1320,25 @@
       </c>
     </row>
     <row r="30" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G30" s="3">
-        <v>1</v>
-      </c>
-      <c r="H30" s="3">
-        <v>-0.5</v>
-      </c>
-      <c r="I30" s="4">
-        <v>2.67649853070782</v>
-      </c>
+      <c r="G30" s="10">
+        <v>1</v>
+      </c>
+      <c r="H30" s="10">
+        <v>-1</v>
+      </c>
+      <c r="I30" s="11">
+        <v>5.4808855554930904</v>
+      </c>
+      <c r="J30" s="11">
+        <v>5.1787166217594098</v>
+      </c>
+      <c r="K30" s="11">
+        <v>5.5241353345395199</v>
+      </c>
+      <c r="L30" s="11">
+        <v>-4.32497790464259E-2</v>
+      </c>
+      <c r="M30" s="4"/>
       <c r="N30" s="1">
         <v>0.2</v>
       </c>
@@ -835,15 +1350,25 @@
       </c>
     </row>
     <row r="31" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G31" s="3">
-        <v>1</v>
-      </c>
-      <c r="H31" s="3">
-        <v>0</v>
-      </c>
-      <c r="I31" s="4">
-        <v>1.2591527832348199</v>
-      </c>
+      <c r="G31" s="10">
+        <v>1</v>
+      </c>
+      <c r="H31" s="10">
+        <v>-0.5</v>
+      </c>
+      <c r="I31" s="11">
+        <v>2.2814474235950901</v>
+      </c>
+      <c r="J31" s="11">
+        <v>2.56701767635067</v>
+      </c>
+      <c r="K31" s="11">
+        <v>2.63534703496846</v>
+      </c>
+      <c r="L31" s="11">
+        <v>-0.353899611373373</v>
+      </c>
+      <c r="M31" s="4"/>
       <c r="N31" s="1">
         <v>0.2</v>
       </c>
@@ -855,15 +1380,25 @@
       </c>
     </row>
     <row r="32" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G32" s="3">
-        <v>1</v>
-      </c>
-      <c r="H32" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="I32" s="4">
-        <v>1.7245752922012201</v>
-      </c>
+      <c r="G32" s="10">
+        <v>1</v>
+      </c>
+      <c r="H32" s="10">
+        <v>0</v>
+      </c>
+      <c r="I32" s="11">
+        <v>1.16328141600171</v>
+      </c>
+      <c r="J32" s="11">
+        <v>0.99737625146296005</v>
+      </c>
+      <c r="K32" s="11">
+        <v>0.87531538856164803</v>
+      </c>
+      <c r="L32" s="11">
+        <v>0.28796602744007099</v>
+      </c>
+      <c r="M32" s="4"/>
       <c r="N32" s="1">
         <v>0.2</v>
       </c>
@@ -875,15 +1410,25 @@
       </c>
     </row>
     <row r="33" spans="7:16" x14ac:dyDescent="0.3">
-      <c r="G33" s="3">
-        <v>1</v>
-      </c>
-      <c r="H33" s="3">
-        <v>1</v>
-      </c>
-      <c r="I33" s="4">
-        <v>4.7141945364464704</v>
-      </c>
+      <c r="G33" s="10">
+        <v>1</v>
+      </c>
+      <c r="H33" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I33" s="11">
+        <v>2.3141535647191902</v>
+      </c>
+      <c r="J33" s="11">
+        <v>1.9277348265752401</v>
+      </c>
+      <c r="K33" s="11">
+        <v>2.0597096151601799</v>
+      </c>
+      <c r="L33" s="11">
+        <v>0.254443949559014</v>
+      </c>
+      <c r="M33" s="4"/>
       <c r="N33" s="1">
         <v>0.2</v>
       </c>
@@ -895,6 +1440,25 @@
       </c>
     </row>
     <row r="34" spans="7:16" x14ac:dyDescent="0.3">
+      <c r="G34" s="10">
+        <v>1</v>
+      </c>
+      <c r="H34" s="10">
+        <v>1</v>
+      </c>
+      <c r="I34" s="11">
+        <v>5.2290907596052403</v>
+      </c>
+      <c r="J34" s="11">
+        <v>4.8160358811665001</v>
+      </c>
+      <c r="K34" s="11">
+        <v>5.1975621974650501</v>
+      </c>
+      <c r="L34" s="11">
+        <v>3.1528562140190099E-2</v>
+      </c>
+      <c r="M34" s="4"/>
       <c r="N34" s="1">
         <v>0.6</v>
       </c>
@@ -1029,5 +1593,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>